<commit_message>
Finished wiring the large components of the Convolution Layer.  Begining to add the detail starting with the Master and Slave Interface signals.  Added Convolutional Layer IP to the vivado project.
</commit_message>
<xml_diff>
--- a/Xilinx_Projects/Thesis_CNN/Controller_registers.xlsx
+++ b/Xilinx_Projects/Thesis_CNN/Controller_registers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marks-M3800\Documents\sensor_to_monitor_node_2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sourcetree_Local\Thesis_VHDL\Xilinx_Projects\Thesis_CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OV5642_Controller" sheetId="1" r:id="rId1"/>
     <sheet name="VGA_Controller" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="90">
   <si>
     <t>diag_reg_0</t>
   </si>
@@ -142,12 +143,165 @@
   </si>
   <si>
     <t>SENSOR REGISTER ADDR[31:24]</t>
+  </si>
+  <si>
+    <t>control_reg</t>
+  </si>
+  <si>
+    <t>enable</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>get_weights</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>weights_loaded</t>
+  </si>
+  <si>
+    <t>Repeat[31:24]</t>
+  </si>
+  <si>
+    <t>Times_repeated[31:24]</t>
+  </si>
+  <si>
+    <t>input_data_addr_reg</t>
+  </si>
+  <si>
+    <t>input_data_addr[7:0]</t>
+  </si>
+  <si>
+    <t>input_data_addr[15:8]</t>
+  </si>
+  <si>
+    <t>input_data_addr[23:16]</t>
+  </si>
+  <si>
+    <t>input_data_addr[31:24]</t>
+  </si>
+  <si>
+    <t>output_data_addr_reg</t>
+  </si>
+  <si>
+    <t>output_data_addr[31:24]</t>
+  </si>
+  <si>
+    <t>output_data_addr[23:16]</t>
+  </si>
+  <si>
+    <t>output_data_addr[15:8]</t>
+  </si>
+  <si>
+    <t>output_data_addr[7:0]</t>
+  </si>
+  <si>
+    <t>relu_en</t>
+  </si>
+  <si>
+    <t>conv_params_reg</t>
+  </si>
+  <si>
+    <t>image_height[31:24]</t>
+  </si>
+  <si>
+    <t>output_volume_height[31:24]</t>
+  </si>
+  <si>
+    <t>image_height[23:16]</t>
+  </si>
+  <si>
+    <t>image_width[15:8]</t>
+  </si>
+  <si>
+    <t>image_width[7:0]</t>
+  </si>
+  <si>
+    <t>image_params_reg</t>
+  </si>
+  <si>
+    <t>Pad[3:0]</t>
+  </si>
+  <si>
+    <t>Stride[11:8]</t>
+  </si>
+  <si>
+    <t>output_volume_width[7:0]</t>
+  </si>
+  <si>
+    <t>output_volume_width[15:8]</t>
+  </si>
+  <si>
+    <t>output_volume_height[23:16]</t>
+  </si>
+  <si>
+    <t>weight_filter_size[31:24]</t>
+  </si>
+  <si>
+    <t>number_of_filters[23:16]</t>
+  </si>
+  <si>
+    <t>conv_out_params_reg</t>
+  </si>
+  <si>
+    <t>inbuff_empty</t>
+  </si>
+  <si>
+    <t>inbuff_almost_empty</t>
+  </si>
+  <si>
+    <t>inbuff_prog_empty</t>
+  </si>
+  <si>
+    <t>inbuff_full</t>
+  </si>
+  <si>
+    <t>inbuff_almost_full</t>
+  </si>
+  <si>
+    <t>inbuff_prog_full</t>
+  </si>
+  <si>
+    <t>outbuff_prog_full</t>
+  </si>
+  <si>
+    <t>outbuff_almost_full</t>
+  </si>
+  <si>
+    <t>outbuff_full</t>
+  </si>
+  <si>
+    <t>outbuff_prog_empty</t>
+  </si>
+  <si>
+    <t>outbuff_almost_empty</t>
+  </si>
+  <si>
+    <t>outbuff_empty</t>
+  </si>
+  <si>
+    <t>filter_weights_addr_reg</t>
+  </si>
+  <si>
+    <t>filter_weights_addr[31:24]</t>
+  </si>
+  <si>
+    <t>filter_weights_addr[23:16]</t>
+  </si>
+  <si>
+    <t>filter_weights_addr[15:8]</t>
+  </si>
+  <si>
+    <t>filter_weights_addr[7:0]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -391,11 +545,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -469,6 +647,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,15 +680,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -509,6 +693,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -824,36 +1018,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="U45" sqref="U45"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="K1" s="32" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36"/>
+      <c r="K1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="34"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="39"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
@@ -906,16 +1100,16 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
       <c r="K3" s="12" t="s">
         <v>4</v>
       </c>
@@ -1010,16 +1204,16 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="40"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
       <c r="K6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1114,16 +1308,16 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="42"/>
       <c r="K9" s="12" t="s">
         <v>4</v>
       </c>
@@ -1218,16 +1412,16 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
       <c r="K12" s="12" t="s">
         <v>4</v>
       </c>
@@ -1255,26 +1449,26 @@
     </row>
     <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-      <c r="K16" s="29" t="s">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
+      <c r="K16" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="31"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="36"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
@@ -1339,12 +1533,12 @@
       <c r="D18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
       <c r="K18" s="22" t="s">
         <v>4</v>
       </c>
@@ -1439,16 +1633,16 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="36"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
       <c r="K21" s="22" t="s">
         <v>4</v>
       </c>
@@ -1555,12 +1749,12 @@
       <c r="D24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="36"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="33"/>
       <c r="K24" s="22" t="s">
         <v>4</v>
       </c>
@@ -1655,16 +1849,16 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="36"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
       <c r="K27" s="22" t="s">
         <v>4</v>
       </c>
@@ -1692,26 +1886,26 @@
     </row>
     <row r="29" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
-      <c r="K30" s="32" t="s">
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="39"/>
+      <c r="K30" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="34"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="39"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
@@ -2015,21 +2209,21 @@
       <c r="E38" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="36"/>
-      <c r="K38" s="37" t="s">
+      <c r="G38" s="32"/>
+      <c r="H38" s="33"/>
+      <c r="K38" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35"/>
-      <c r="O38" s="35"/>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="35"/>
-      <c r="R38" s="36"/>
+      <c r="L38" s="32"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="33"/>
     </row>
     <row r="39" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
@@ -2100,49 +2294,49 @@
       </c>
     </row>
     <row r="41" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="36"/>
-      <c r="K41" s="37" t="s">
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="33"/>
+      <c r="K41" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="36"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="33"/>
     </row>
     <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="44" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="31"/>
-      <c r="K44" s="32" t="s">
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="K44" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="33"/>
-      <c r="O44" s="33"/>
-      <c r="P44" s="33"/>
-      <c r="Q44" s="33"/>
-      <c r="R44" s="34"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="39"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
@@ -2219,16 +2413,16 @@
       <c r="H46" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K46" s="37" t="s">
+      <c r="K46" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="35"/>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="35"/>
-      <c r="R46" s="36"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
+      <c r="Q46" s="32"/>
+      <c r="R46" s="33"/>
     </row>
     <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="24"/>
@@ -2323,16 +2517,16 @@
       <c r="H49" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K49" s="37" t="s">
+      <c r="K49" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35"/>
-      <c r="O49" s="35"/>
-      <c r="P49" s="35"/>
-      <c r="Q49" s="35"/>
-      <c r="R49" s="36"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="32"/>
+      <c r="O49" s="32"/>
+      <c r="P49" s="32"/>
+      <c r="Q49" s="32"/>
+      <c r="R49" s="33"/>
     </row>
     <row r="50" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="24"/>
@@ -2427,16 +2621,16 @@
       <c r="H52" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="K52" s="37" t="s">
+      <c r="K52" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="L52" s="35"/>
-      <c r="M52" s="35"/>
-      <c r="N52" s="35"/>
-      <c r="O52" s="35"/>
-      <c r="P52" s="35"/>
-      <c r="Q52" s="35"/>
-      <c r="R52" s="36"/>
+      <c r="L52" s="32"/>
+      <c r="M52" s="32"/>
+      <c r="N52" s="32"/>
+      <c r="O52" s="32"/>
+      <c r="P52" s="32"/>
+      <c r="Q52" s="32"/>
+      <c r="R52" s="33"/>
     </row>
     <row r="53" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="24"/>
@@ -2531,29 +2725,29 @@
       <c r="H55" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K55" s="37" t="s">
+      <c r="K55" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="L55" s="35"/>
-      <c r="M55" s="35"/>
-      <c r="N55" s="35"/>
-      <c r="O55" s="35"/>
-      <c r="P55" s="35"/>
-      <c r="Q55" s="35"/>
-      <c r="R55" s="36"/>
+      <c r="L55" s="32"/>
+      <c r="M55" s="32"/>
+      <c r="N55" s="32"/>
+      <c r="O55" s="32"/>
+      <c r="P55" s="32"/>
+      <c r="Q55" s="32"/>
+      <c r="R55" s="33"/>
     </row>
     <row r="58" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="59" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="31"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="36"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
@@ -2731,15 +2925,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="K52:R52"/>
-    <mergeCell ref="K55:R55"/>
-    <mergeCell ref="K49:R49"/>
-    <mergeCell ref="K46:R46"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="K30:R30"/>
-    <mergeCell ref="K41:R41"/>
-    <mergeCell ref="K38:R38"/>
-    <mergeCell ref="K44:R44"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="K1:R1"/>
     <mergeCell ref="K16:R16"/>
@@ -2756,6 +2941,15 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A12:H12"/>
+    <mergeCell ref="K52:R52"/>
+    <mergeCell ref="K55:R55"/>
+    <mergeCell ref="K49:R49"/>
+    <mergeCell ref="K46:R46"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="K30:R30"/>
+    <mergeCell ref="K41:R41"/>
+    <mergeCell ref="K38:R38"/>
+    <mergeCell ref="K44:R44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2763,26 +2957,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection sqref="A1:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
@@ -3024,16 +3218,16 @@
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
@@ -3273,16 +3467,16 @@
     </row>
     <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="36"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
@@ -3329,10 +3523,10 @@
       <c r="F31" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="41" t="s">
+      <c r="G31" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="42"/>
+      <c r="H31" s="44"/>
     </row>
     <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
@@ -3371,16 +3565,16 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="36"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
@@ -3437,10 +3631,10 @@
       <c r="F37" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="41" t="s">
+      <c r="G37" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="H37" s="42"/>
+      <c r="H37" s="44"/>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
@@ -3479,29 +3673,29 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="36"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="33"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="31"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="36"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
@@ -3754,4 +3948,1626 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061DCDF6-B37A-4793-844B-0A18FAFEE277}">
+  <dimension ref="A1:R55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39"/>
+      <c r="K1" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="39"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>31</v>
+      </c>
+      <c r="B2" s="8">
+        <v>30</v>
+      </c>
+      <c r="C2" s="8">
+        <v>29</v>
+      </c>
+      <c r="D2" s="8">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8">
+        <v>27</v>
+      </c>
+      <c r="F2" s="8">
+        <v>26</v>
+      </c>
+      <c r="G2" s="8">
+        <v>25</v>
+      </c>
+      <c r="H2" s="9">
+        <v>24</v>
+      </c>
+      <c r="K2" s="7">
+        <v>31</v>
+      </c>
+      <c r="L2" s="8">
+        <v>30</v>
+      </c>
+      <c r="M2" s="8">
+        <v>29</v>
+      </c>
+      <c r="N2" s="8">
+        <v>28</v>
+      </c>
+      <c r="O2" s="8">
+        <v>27</v>
+      </c>
+      <c r="P2" s="8">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>25</v>
+      </c>
+      <c r="R2" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="44"/>
+      <c r="K3" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="44"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>23</v>
+      </c>
+      <c r="B5" s="8">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8">
+        <v>21</v>
+      </c>
+      <c r="D5" s="8">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8">
+        <v>17</v>
+      </c>
+      <c r="H5" s="9">
+        <v>16</v>
+      </c>
+      <c r="K5" s="7">
+        <v>23</v>
+      </c>
+      <c r="L5" s="8">
+        <v>22</v>
+      </c>
+      <c r="M5" s="8">
+        <v>21</v>
+      </c>
+      <c r="N5" s="8">
+        <v>20</v>
+      </c>
+      <c r="O5" s="8">
+        <v>19</v>
+      </c>
+      <c r="P5" s="8">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>17</v>
+      </c>
+      <c r="R5" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="44"/>
+    </row>
+    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8">
+        <v>13</v>
+      </c>
+      <c r="D8" s="8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="8">
+        <v>11</v>
+      </c>
+      <c r="F8" s="8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="8">
+        <v>9</v>
+      </c>
+      <c r="H8" s="9">
+        <v>8</v>
+      </c>
+      <c r="K8" s="7">
+        <v>15</v>
+      </c>
+      <c r="L8" s="8">
+        <v>14</v>
+      </c>
+      <c r="M8" s="8">
+        <v>13</v>
+      </c>
+      <c r="N8" s="8">
+        <v>12</v>
+      </c>
+      <c r="O8" s="8">
+        <v>11</v>
+      </c>
+      <c r="P8" s="8">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>9</v>
+      </c>
+      <c r="R8" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="44"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="6"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8">
+        <v>6</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8">
+        <v>3</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>7</v>
+      </c>
+      <c r="L11" s="8">
+        <v>6</v>
+      </c>
+      <c r="M11" s="8">
+        <v>5</v>
+      </c>
+      <c r="N11" s="8">
+        <v>4</v>
+      </c>
+      <c r="O11" s="8">
+        <v>3</v>
+      </c>
+      <c r="P11" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>1</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="44"/>
+    </row>
+    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
+      <c r="K15" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="39"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>31</v>
+      </c>
+      <c r="B16" s="8">
+        <v>30</v>
+      </c>
+      <c r="C16" s="8">
+        <v>29</v>
+      </c>
+      <c r="D16" s="8">
+        <v>28</v>
+      </c>
+      <c r="E16" s="8">
+        <v>27</v>
+      </c>
+      <c r="F16" s="8">
+        <v>26</v>
+      </c>
+      <c r="G16" s="8">
+        <v>25</v>
+      </c>
+      <c r="H16" s="9">
+        <v>24</v>
+      </c>
+      <c r="K16" s="7">
+        <v>31</v>
+      </c>
+      <c r="L16" s="8">
+        <v>30</v>
+      </c>
+      <c r="M16" s="8">
+        <v>29</v>
+      </c>
+      <c r="N16" s="8">
+        <v>28</v>
+      </c>
+      <c r="O16" s="8">
+        <v>27</v>
+      </c>
+      <c r="P16" s="8">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>25</v>
+      </c>
+      <c r="R16" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="44"/>
+      <c r="K17" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="44"/>
+    </row>
+    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="6"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>23</v>
+      </c>
+      <c r="B19" s="8">
+        <v>22</v>
+      </c>
+      <c r="C19" s="8">
+        <v>21</v>
+      </c>
+      <c r="D19" s="8">
+        <v>20</v>
+      </c>
+      <c r="E19" s="8">
+        <v>19</v>
+      </c>
+      <c r="F19" s="8">
+        <v>18</v>
+      </c>
+      <c r="G19" s="8">
+        <v>17</v>
+      </c>
+      <c r="H19" s="9">
+        <v>16</v>
+      </c>
+      <c r="K19" s="7">
+        <v>23</v>
+      </c>
+      <c r="L19" s="8">
+        <v>22</v>
+      </c>
+      <c r="M19" s="8">
+        <v>21</v>
+      </c>
+      <c r="N19" s="8">
+        <v>20</v>
+      </c>
+      <c r="O19" s="8">
+        <v>19</v>
+      </c>
+      <c r="P19" s="8">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>17</v>
+      </c>
+      <c r="R19" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="44"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="6"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>15</v>
+      </c>
+      <c r="B22" s="8">
+        <v>14</v>
+      </c>
+      <c r="C22" s="8">
+        <v>13</v>
+      </c>
+      <c r="D22" s="8">
+        <v>12</v>
+      </c>
+      <c r="E22" s="8">
+        <v>11</v>
+      </c>
+      <c r="F22" s="8">
+        <v>10</v>
+      </c>
+      <c r="G22" s="8">
+        <v>9</v>
+      </c>
+      <c r="H22" s="9">
+        <v>8</v>
+      </c>
+      <c r="K22" s="7">
+        <v>15</v>
+      </c>
+      <c r="L22" s="8">
+        <v>14</v>
+      </c>
+      <c r="M22" s="8">
+        <v>13</v>
+      </c>
+      <c r="N22" s="8">
+        <v>12</v>
+      </c>
+      <c r="O22" s="8">
+        <v>11</v>
+      </c>
+      <c r="P22" s="8">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>9</v>
+      </c>
+      <c r="R22" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="44"/>
+    </row>
+    <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="6"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>7</v>
+      </c>
+      <c r="B25" s="8">
+        <v>6</v>
+      </c>
+      <c r="C25" s="8">
+        <v>5</v>
+      </c>
+      <c r="D25" s="8">
+        <v>4</v>
+      </c>
+      <c r="E25" s="8">
+        <v>3</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="K25" s="7">
+        <v>7</v>
+      </c>
+      <c r="L25" s="8">
+        <v>6</v>
+      </c>
+      <c r="M25" s="8">
+        <v>5</v>
+      </c>
+      <c r="N25" s="8">
+        <v>4</v>
+      </c>
+      <c r="O25" s="8">
+        <v>3</v>
+      </c>
+      <c r="P25" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>1</v>
+      </c>
+      <c r="R25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="44"/>
+    </row>
+    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
+      <c r="K29" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="39"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>31</v>
+      </c>
+      <c r="B30" s="8">
+        <v>30</v>
+      </c>
+      <c r="C30" s="8">
+        <v>29</v>
+      </c>
+      <c r="D30" s="8">
+        <v>28</v>
+      </c>
+      <c r="E30" s="8">
+        <v>27</v>
+      </c>
+      <c r="F30" s="8">
+        <v>26</v>
+      </c>
+      <c r="G30" s="8">
+        <v>25</v>
+      </c>
+      <c r="H30" s="9">
+        <v>24</v>
+      </c>
+      <c r="K30" s="7">
+        <v>31</v>
+      </c>
+      <c r="L30" s="8">
+        <v>30</v>
+      </c>
+      <c r="M30" s="8">
+        <v>29</v>
+      </c>
+      <c r="N30" s="8">
+        <v>28</v>
+      </c>
+      <c r="O30" s="8">
+        <v>27</v>
+      </c>
+      <c r="P30" s="8">
+        <v>26</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>25</v>
+      </c>
+      <c r="R30" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="44"/>
+      <c r="K31" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="44"/>
+    </row>
+    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="6"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>23</v>
+      </c>
+      <c r="B33" s="8">
+        <v>22</v>
+      </c>
+      <c r="C33" s="8">
+        <v>21</v>
+      </c>
+      <c r="D33" s="8">
+        <v>20</v>
+      </c>
+      <c r="E33" s="8">
+        <v>19</v>
+      </c>
+      <c r="F33" s="8">
+        <v>18</v>
+      </c>
+      <c r="G33" s="8">
+        <v>17</v>
+      </c>
+      <c r="H33" s="9">
+        <v>16</v>
+      </c>
+      <c r="K33" s="7">
+        <v>23</v>
+      </c>
+      <c r="L33" s="8">
+        <v>22</v>
+      </c>
+      <c r="M33" s="8">
+        <v>21</v>
+      </c>
+      <c r="N33" s="8">
+        <v>20</v>
+      </c>
+      <c r="O33" s="8">
+        <v>19</v>
+      </c>
+      <c r="P33" s="8">
+        <v>18</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>17</v>
+      </c>
+      <c r="R33" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="44"/>
+      <c r="K34" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="46"/>
+      <c r="O34" s="46"/>
+      <c r="P34" s="46"/>
+      <c r="Q34" s="46"/>
+      <c r="R34" s="44"/>
+    </row>
+    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="6"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="6"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>15</v>
+      </c>
+      <c r="B36" s="8">
+        <v>14</v>
+      </c>
+      <c r="C36" s="8">
+        <v>13</v>
+      </c>
+      <c r="D36" s="8">
+        <v>12</v>
+      </c>
+      <c r="E36" s="8">
+        <v>11</v>
+      </c>
+      <c r="F36" s="8">
+        <v>10</v>
+      </c>
+      <c r="G36" s="8">
+        <v>9</v>
+      </c>
+      <c r="H36" s="9">
+        <v>8</v>
+      </c>
+      <c r="K36" s="7">
+        <v>15</v>
+      </c>
+      <c r="L36" s="8">
+        <v>14</v>
+      </c>
+      <c r="M36" s="8">
+        <v>13</v>
+      </c>
+      <c r="N36" s="8">
+        <v>12</v>
+      </c>
+      <c r="O36" s="8">
+        <v>11</v>
+      </c>
+      <c r="P36" s="8">
+        <v>10</v>
+      </c>
+      <c r="Q36" s="8">
+        <v>9</v>
+      </c>
+      <c r="R36" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="44"/>
+      <c r="K37" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="44"/>
+    </row>
+    <row r="38" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="6"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="6"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>7</v>
+      </c>
+      <c r="B39" s="8">
+        <v>6</v>
+      </c>
+      <c r="C39" s="8">
+        <v>5</v>
+      </c>
+      <c r="D39" s="8">
+        <v>4</v>
+      </c>
+      <c r="E39" s="8">
+        <v>3</v>
+      </c>
+      <c r="F39" s="8">
+        <v>2</v>
+      </c>
+      <c r="G39" s="8">
+        <v>1</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0</v>
+      </c>
+      <c r="K39" s="7">
+        <v>7</v>
+      </c>
+      <c r="L39" s="8">
+        <v>6</v>
+      </c>
+      <c r="M39" s="8">
+        <v>5</v>
+      </c>
+      <c r="N39" s="8">
+        <v>4</v>
+      </c>
+      <c r="O39" s="8">
+        <v>3</v>
+      </c>
+      <c r="P39" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>1</v>
+      </c>
+      <c r="R39" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="44"/>
+      <c r="K40" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="46"/>
+      <c r="P40" s="46"/>
+      <c r="Q40" s="46"/>
+      <c r="R40" s="44"/>
+    </row>
+    <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="39"/>
+      <c r="K43" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="39"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>31</v>
+      </c>
+      <c r="B44" s="8">
+        <v>30</v>
+      </c>
+      <c r="C44" s="8">
+        <v>29</v>
+      </c>
+      <c r="D44" s="8">
+        <v>28</v>
+      </c>
+      <c r="E44" s="8">
+        <v>27</v>
+      </c>
+      <c r="F44" s="8">
+        <v>26</v>
+      </c>
+      <c r="G44" s="8">
+        <v>25</v>
+      </c>
+      <c r="H44" s="9">
+        <v>24</v>
+      </c>
+      <c r="K44" s="7">
+        <v>31</v>
+      </c>
+      <c r="L44" s="8">
+        <v>30</v>
+      </c>
+      <c r="M44" s="8">
+        <v>29</v>
+      </c>
+      <c r="N44" s="8">
+        <v>28</v>
+      </c>
+      <c r="O44" s="8">
+        <v>27</v>
+      </c>
+      <c r="P44" s="8">
+        <v>26</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>25</v>
+      </c>
+      <c r="R44" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="44"/>
+      <c r="K45" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="L45" s="46"/>
+      <c r="M45" s="46"/>
+      <c r="N45" s="46"/>
+      <c r="O45" s="46"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="44"/>
+    </row>
+    <row r="46" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="6"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="6"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
+        <v>23</v>
+      </c>
+      <c r="B47" s="8">
+        <v>22</v>
+      </c>
+      <c r="C47" s="8">
+        <v>21</v>
+      </c>
+      <c r="D47" s="8">
+        <v>20</v>
+      </c>
+      <c r="E47" s="8">
+        <v>19</v>
+      </c>
+      <c r="F47" s="8">
+        <v>18</v>
+      </c>
+      <c r="G47" s="8">
+        <v>17</v>
+      </c>
+      <c r="H47" s="9">
+        <v>16</v>
+      </c>
+      <c r="K47" s="7">
+        <v>23</v>
+      </c>
+      <c r="L47" s="8">
+        <v>22</v>
+      </c>
+      <c r="M47" s="8">
+        <v>21</v>
+      </c>
+      <c r="N47" s="8">
+        <v>20</v>
+      </c>
+      <c r="O47" s="8">
+        <v>19</v>
+      </c>
+      <c r="P47" s="8">
+        <v>18</v>
+      </c>
+      <c r="Q47" s="8">
+        <v>17</v>
+      </c>
+      <c r="R47" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="46"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="44"/>
+      <c r="K48" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="L48" s="46"/>
+      <c r="M48" s="46"/>
+      <c r="N48" s="46"/>
+      <c r="O48" s="46"/>
+      <c r="P48" s="46"/>
+      <c r="Q48" s="46"/>
+      <c r="R48" s="44"/>
+    </row>
+    <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="6"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="6"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
+        <v>15</v>
+      </c>
+      <c r="B50" s="8">
+        <v>14</v>
+      </c>
+      <c r="C50" s="8">
+        <v>13</v>
+      </c>
+      <c r="D50" s="8">
+        <v>12</v>
+      </c>
+      <c r="E50" s="8">
+        <v>11</v>
+      </c>
+      <c r="F50" s="8">
+        <v>10</v>
+      </c>
+      <c r="G50" s="8">
+        <v>9</v>
+      </c>
+      <c r="H50" s="9">
+        <v>8</v>
+      </c>
+      <c r="K50" s="7">
+        <v>15</v>
+      </c>
+      <c r="L50" s="8">
+        <v>14</v>
+      </c>
+      <c r="M50" s="8">
+        <v>13</v>
+      </c>
+      <c r="N50" s="8">
+        <v>12</v>
+      </c>
+      <c r="O50" s="8">
+        <v>11</v>
+      </c>
+      <c r="P50" s="8">
+        <v>10</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>9</v>
+      </c>
+      <c r="R50" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="44"/>
+      <c r="K51" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M51" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N51" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="O51" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="P51" s="46"/>
+      <c r="Q51" s="46"/>
+      <c r="R51" s="44"/>
+    </row>
+    <row r="52" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="6"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="6"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A53" s="7">
+        <v>7</v>
+      </c>
+      <c r="B53" s="8">
+        <v>6</v>
+      </c>
+      <c r="C53" s="8">
+        <v>5</v>
+      </c>
+      <c r="D53" s="8">
+        <v>4</v>
+      </c>
+      <c r="E53" s="8">
+        <v>3</v>
+      </c>
+      <c r="F53" s="8">
+        <v>2</v>
+      </c>
+      <c r="G53" s="8">
+        <v>1</v>
+      </c>
+      <c r="H53" s="9">
+        <v>0</v>
+      </c>
+      <c r="K53" s="7">
+        <v>7</v>
+      </c>
+      <c r="L53" s="8">
+        <v>6</v>
+      </c>
+      <c r="M53" s="8">
+        <v>5</v>
+      </c>
+      <c r="N53" s="8">
+        <v>4</v>
+      </c>
+      <c r="O53" s="8">
+        <v>3</v>
+      </c>
+      <c r="P53" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>1</v>
+      </c>
+      <c r="R53" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="44"/>
+      <c r="K54" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M54" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N54" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="O54" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="P54" s="46"/>
+      <c r="Q54" s="46"/>
+      <c r="R54" s="44"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E55" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="K48:R48"/>
+    <mergeCell ref="K43:R43"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="O54:R54"/>
+    <mergeCell ref="O51:R51"/>
+    <mergeCell ref="K31:R31"/>
+    <mergeCell ref="K34:R34"/>
+    <mergeCell ref="K37:R37"/>
+    <mergeCell ref="K40:R40"/>
+    <mergeCell ref="K15:R15"/>
+    <mergeCell ref="K17:R17"/>
+    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K26:R26"/>
+    <mergeCell ref="K29:R29"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A31:H31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Beginning detailed design with the filter weight fetching operations.  Investigating Alexnet weights from tensorflow to develop uploadable filter weight file. Plan is to get the pretrained weights from tensorflow or caffe and then put those value into a text file i can then upload to the DDR memory on the Nexys board.
</commit_message>
<xml_diff>
--- a/Xilinx_Projects/Thesis_CNN/Controller_registers.xlsx
+++ b/Xilinx_Projects/Thesis_CNN/Controller_registers.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OV5642_Controller" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="96">
   <si>
     <t>diag_reg_0</t>
   </si>
@@ -296,12 +296,30 @@
   </si>
   <si>
     <t>filter_weights_addr[7:0]</t>
+  </si>
+  <si>
+    <t>Layer_Number[23:16]</t>
+  </si>
+  <si>
+    <t>filter_weights_bytes_reg</t>
+  </si>
+  <si>
+    <t>filter_weights_bytes[31:24]</t>
+  </si>
+  <si>
+    <t>filter_weights_bytes[23:16]</t>
+  </si>
+  <si>
+    <t>filter_weights_bytes[15:8]</t>
+  </si>
+  <si>
+    <t>filter_weights_bytes[7:0]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -653,13 +671,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -678,6 +694,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -699,10 +724,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1018,7 +1039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
@@ -1100,16 +1121,16 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
       <c r="K3" s="12" t="s">
         <v>4</v>
       </c>
@@ -1204,16 +1225,16 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="45"/>
       <c r="K6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1308,16 +1329,16 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="42"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
       <c r="K9" s="12" t="s">
         <v>4</v>
       </c>
@@ -1412,16 +1433,16 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45"/>
       <c r="K12" s="12" t="s">
         <v>4</v>
       </c>
@@ -1533,12 +1554,12 @@
       <c r="D18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="33"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="41"/>
       <c r="K18" s="22" t="s">
         <v>4</v>
       </c>
@@ -1633,16 +1654,16 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="41"/>
       <c r="K21" s="22" t="s">
         <v>4</v>
       </c>
@@ -1749,12 +1770,12 @@
       <c r="D24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="33"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="41"/>
       <c r="K24" s="22" t="s">
         <v>4</v>
       </c>
@@ -1849,16 +1870,16 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="33"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="41"/>
       <c r="K27" s="22" t="s">
         <v>4</v>
       </c>
@@ -2209,21 +2230,21 @@
       <c r="E38" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="32"/>
-      <c r="H38" s="33"/>
-      <c r="K38" s="31" t="s">
+      <c r="G38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="K38" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32"/>
-      <c r="R38" s="33"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="40"/>
+      <c r="P38" s="40"/>
+      <c r="Q38" s="40"/>
+      <c r="R38" s="41"/>
     </row>
     <row r="39" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
@@ -2294,26 +2315,26 @@
       </c>
     </row>
     <row r="41" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="33"/>
-      <c r="K41" s="31" t="s">
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="41"/>
+      <c r="K41" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="33"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="40"/>
+      <c r="N41" s="40"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="40"/>
+      <c r="R41" s="41"/>
     </row>
     <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="44" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2413,16 +2434,16 @@
       <c r="H46" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K46" s="31" t="s">
+      <c r="K46" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="32"/>
-      <c r="R46" s="33"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="40"/>
+      <c r="O46" s="40"/>
+      <c r="P46" s="40"/>
+      <c r="Q46" s="40"/>
+      <c r="R46" s="41"/>
     </row>
     <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="24"/>
@@ -2517,16 +2538,16 @@
       <c r="H49" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K49" s="31" t="s">
+      <c r="K49" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="32"/>
-      <c r="R49" s="33"/>
+      <c r="L49" s="40"/>
+      <c r="M49" s="40"/>
+      <c r="N49" s="40"/>
+      <c r="O49" s="40"/>
+      <c r="P49" s="40"/>
+      <c r="Q49" s="40"/>
+      <c r="R49" s="41"/>
     </row>
     <row r="50" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="24"/>
@@ -2621,16 +2642,16 @@
       <c r="H52" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="K52" s="31" t="s">
+      <c r="K52" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="L52" s="32"/>
-      <c r="M52" s="32"/>
-      <c r="N52" s="32"/>
-      <c r="O52" s="32"/>
-      <c r="P52" s="32"/>
-      <c r="Q52" s="32"/>
-      <c r="R52" s="33"/>
+      <c r="L52" s="40"/>
+      <c r="M52" s="40"/>
+      <c r="N52" s="40"/>
+      <c r="O52" s="40"/>
+      <c r="P52" s="40"/>
+      <c r="Q52" s="40"/>
+      <c r="R52" s="41"/>
     </row>
     <row r="53" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="24"/>
@@ -2725,16 +2746,16 @@
       <c r="H55" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K55" s="31" t="s">
+      <c r="K55" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="L55" s="32"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="32"/>
-      <c r="O55" s="32"/>
-      <c r="P55" s="32"/>
-      <c r="Q55" s="32"/>
-      <c r="R55" s="33"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+      <c r="O55" s="40"/>
+      <c r="P55" s="40"/>
+      <c r="Q55" s="40"/>
+      <c r="R55" s="41"/>
     </row>
     <row r="58" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="59" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2925,6 +2946,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="K52:R52"/>
+    <mergeCell ref="K55:R55"/>
+    <mergeCell ref="K49:R49"/>
+    <mergeCell ref="K46:R46"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="K30:R30"/>
+    <mergeCell ref="K41:R41"/>
+    <mergeCell ref="K38:R38"/>
+    <mergeCell ref="K44:R44"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="K1:R1"/>
     <mergeCell ref="K16:R16"/>
@@ -2941,15 +2971,6 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A12:H12"/>
-    <mergeCell ref="K52:R52"/>
-    <mergeCell ref="K55:R55"/>
-    <mergeCell ref="K49:R49"/>
-    <mergeCell ref="K46:R46"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="K30:R30"/>
-    <mergeCell ref="K41:R41"/>
-    <mergeCell ref="K38:R38"/>
-    <mergeCell ref="K44:R44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2957,7 +2978,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3523,10 +3544,10 @@
       <c r="F31" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="43" t="s">
+      <c r="G31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="44"/>
+      <c r="H31" s="47"/>
     </row>
     <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
@@ -3565,16 +3586,16 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="33"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="41"/>
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
@@ -3631,10 +3652,10 @@
       <c r="F37" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="43" t="s">
+      <c r="G37" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H37" s="44"/>
+      <c r="H37" s="47"/>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
@@ -3673,16 +3694,16 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="33"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="41"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3951,11 +3972,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061DCDF6-B37A-4793-844B-0A18FAFEE277}">
-  <dimension ref="A1:R55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="H43" workbookViewId="0">
+      <selection activeCell="P69" sqref="P69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3968,7 +3989,7 @@
     <col min="8" max="8" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
         <v>39</v>
       </c>
@@ -3989,8 +4010,18 @@
       <c r="P1" s="38"/>
       <c r="Q1" s="38"/>
       <c r="R1" s="39"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="U1" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="39"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>31</v>
       </c>
@@ -4039,30 +4070,64 @@
       <c r="R2" s="9">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45" t="s">
+      <c r="U2" s="7">
+        <v>31</v>
+      </c>
+      <c r="V2" s="8">
+        <v>30</v>
+      </c>
+      <c r="W2" s="8">
+        <v>29</v>
+      </c>
+      <c r="X2" s="8">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>26</v>
+      </c>
+      <c r="AA2" s="8">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="44"/>
-      <c r="K3" s="45" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="47"/>
+      <c r="K3" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="44"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="47"/>
+      <c r="U3" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="47"/>
+    </row>
+    <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4079,8 +4144,16 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="6"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="U4" s="4"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="6"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>23</v>
       </c>
@@ -4129,44 +4202,64 @@
       <c r="R5" s="9">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="45" t="s">
+      <c r="U5" s="7">
+        <v>23</v>
+      </c>
+      <c r="V5" s="8">
+        <v>22</v>
+      </c>
+      <c r="W5" s="8">
+        <v>21</v>
+      </c>
+      <c r="X5" s="8">
+        <v>20</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>18</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>17</v>
+      </c>
+      <c r="AB5" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="47"/>
+      <c r="K6" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="44"/>
-    </row>
-    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="47"/>
+      <c r="U6" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="49"/>
+      <c r="AB6" s="47"/>
+    </row>
+    <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -4183,8 +4276,16 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="6"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="U7" s="4"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="6"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>15</v>
       </c>
@@ -4233,8 +4334,32 @@
       <c r="R8" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U8" s="7">
+        <v>15</v>
+      </c>
+      <c r="V8" s="8">
+        <v>14</v>
+      </c>
+      <c r="W8" s="8">
+        <v>13</v>
+      </c>
+      <c r="X8" s="8">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>11</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="8">
+        <v>9</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -4245,7 +4370,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>4</v>
@@ -4257,20 +4382,30 @@
         <v>4</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="44"/>
-    </row>
-    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="47"/>
+      <c r="U9" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="47"/>
+    </row>
+    <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -4287,8 +4422,16 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="6"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="U10" s="4"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="6"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>7</v>
       </c>
@@ -4337,8 +4480,32 @@
       <c r="R11" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U11" s="7">
+        <v>7</v>
+      </c>
+      <c r="V11" s="8">
+        <v>6</v>
+      </c>
+      <c r="W11" s="8">
+        <v>5</v>
+      </c>
+      <c r="X11" s="8">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="8">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="8">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>4</v>
       </c>
@@ -4349,33 +4516,43 @@
         <v>4</v>
       </c>
       <c r="D12" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>4</v>
+      <c r="G12" s="31" t="s">
+        <v>19</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="45" t="s">
+      <c r="K12" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="44"/>
-    </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="47"/>
+      <c r="U12" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="47"/>
+    </row>
+    <row r="14" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
         <v>20</v>
       </c>
@@ -4397,7 +4574,7 @@
       <c r="Q15" s="38"/>
       <c r="R15" s="39"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>31</v>
       </c>
@@ -4448,26 +4625,26 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="44"/>
-      <c r="K17" s="45" t="s">
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="47"/>
+      <c r="K17" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="44"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="47"/>
     </row>
     <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
@@ -4482,7 +4659,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
-      <c r="O18" s="48"/>
+      <c r="O18" s="33"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="6"/>
@@ -4562,16 +4739,16 @@
       <c r="H20" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="K20" s="45" t="s">
+      <c r="K20" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="46"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="44"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="47"/>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
@@ -4666,16 +4843,16 @@
       <c r="H23" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="K23" s="45" t="s">
+      <c r="K23" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="44"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="47"/>
     </row>
     <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
@@ -4770,16 +4947,16 @@
       <c r="H26" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="K26" s="45" t="s">
+      <c r="K26" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="44"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="47"/>
     </row>
     <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4855,26 +5032,26 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="44"/>
-      <c r="K31" s="45" t="s">
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="47"/>
+      <c r="K31" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="46"/>
-      <c r="Q31" s="46"/>
-      <c r="R31" s="44"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="47"/>
     </row>
     <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
@@ -4945,26 +5122,26 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="44"/>
-      <c r="K34" s="45" t="s">
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="47"/>
+      <c r="K34" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="L34" s="46"/>
-      <c r="M34" s="46"/>
-      <c r="N34" s="46"/>
-      <c r="O34" s="46"/>
-      <c r="P34" s="46"/>
-      <c r="Q34" s="46"/>
-      <c r="R34" s="44"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="47"/>
     </row>
     <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
@@ -5035,26 +5212,26 @@
       </c>
     </row>
     <row r="37" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="44"/>
-      <c r="K37" s="45" t="s">
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="47"/>
+      <c r="K37" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="44"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="47"/>
     </row>
     <row r="38" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
@@ -5125,26 +5302,26 @@
       </c>
     </row>
     <row r="40" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="44"/>
-      <c r="K40" s="45" t="s">
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="47"/>
+      <c r="K40" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="L40" s="46"/>
-      <c r="M40" s="46"/>
-      <c r="N40" s="46"/>
-      <c r="O40" s="46"/>
-      <c r="P40" s="46"/>
-      <c r="Q40" s="46"/>
-      <c r="R40" s="44"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="47"/>
     </row>
     <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -5220,26 +5397,26 @@
       </c>
     </row>
     <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="44"/>
-      <c r="K45" s="45" t="s">
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="47"/>
+      <c r="K45" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="L45" s="46"/>
-      <c r="M45" s="46"/>
-      <c r="N45" s="46"/>
-      <c r="O45" s="46"/>
-      <c r="P45" s="46"/>
-      <c r="Q45" s="46"/>
-      <c r="R45" s="44"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49"/>
+      <c r="Q45" s="49"/>
+      <c r="R45" s="47"/>
     </row>
     <row r="46" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
@@ -5310,26 +5487,26 @@
       </c>
     </row>
     <row r="48" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="46"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="46"/>
-      <c r="H48" s="44"/>
-      <c r="K48" s="45" t="s">
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="47"/>
+      <c r="K48" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="L48" s="46"/>
-      <c r="M48" s="46"/>
-      <c r="N48" s="46"/>
-      <c r="O48" s="46"/>
-      <c r="P48" s="46"/>
-      <c r="Q48" s="46"/>
-      <c r="R48" s="44"/>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+      <c r="O48" s="49"/>
+      <c r="P48" s="49"/>
+      <c r="Q48" s="49"/>
+      <c r="R48" s="47"/>
     </row>
     <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4"/>
@@ -5400,16 +5577,16 @@
       </c>
     </row>
     <row r="51" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="46"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="46"/>
-      <c r="G51" s="46"/>
-      <c r="H51" s="44"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="47"/>
       <c r="K51" s="12" t="s">
         <v>4</v>
       </c>
@@ -5422,12 +5599,12 @@
       <c r="N51" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O51" s="43" t="s">
+      <c r="O51" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="P51" s="46"/>
-      <c r="Q51" s="46"/>
-      <c r="R51" s="44"/>
+      <c r="P51" s="49"/>
+      <c r="Q51" s="49"/>
+      <c r="R51" s="47"/>
     </row>
     <row r="52" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
@@ -5498,16 +5675,16 @@
       </c>
     </row>
     <row r="54" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="46"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="46"/>
-      <c r="H54" s="44"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="47"/>
       <c r="K54" s="12" t="s">
         <v>4</v>
       </c>
@@ -5520,23 +5697,43 @@
       <c r="N54" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O54" s="43" t="s">
+      <c r="O54" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="P54" s="46"/>
-      <c r="Q54" s="46"/>
-      <c r="R54" s="44"/>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
+      <c r="R54" s="47"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E55" s="47"/>
+      <c r="E55" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="K48:R48"/>
-    <mergeCell ref="K43:R43"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="O54:R54"/>
-    <mergeCell ref="O51:R51"/>
+  <mergeCells count="40">
+    <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="U6:AB6"/>
+    <mergeCell ref="U9:AB9"/>
+    <mergeCell ref="U12:AB12"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A54:H54"/>
     <mergeCell ref="K31:R31"/>
     <mergeCell ref="K34:R34"/>
     <mergeCell ref="K37:R37"/>
@@ -5547,25 +5744,11 @@
     <mergeCell ref="K23:R23"/>
     <mergeCell ref="K26:R26"/>
     <mergeCell ref="K29:R29"/>
-    <mergeCell ref="A43:H43"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A54:H54"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="K48:R48"/>
+    <mergeCell ref="K43:R43"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="O54:R54"/>
+    <mergeCell ref="O51:R51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Cleaned up the Slave Interface Xilinx Code to output wd and we signals.   Began editing the Master Interface code to handle reading weights, reading input image, and writing the output volume to memory.  Master Interface needs more work
To Do:
- Complete first pass of Master Interface
- Move on to edit the Convolution Controller code.
</commit_message>
<xml_diff>
--- a/Xilinx_Projects/Thesis_CNN/Controller_registers.xlsx
+++ b/Xilinx_Projects/Thesis_CNN/Controller_registers.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OV5642_Controller" sheetId="1" r:id="rId1"/>
     <sheet name="VGA_Controller" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Conv_Controller" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -319,7 +320,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -678,6 +679,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -694,15 +704,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1039,7 +1040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
@@ -1049,26 +1050,26 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36"/>
-      <c r="K1" s="37" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39"/>
+      <c r="K1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="39"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="42"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
@@ -1470,26 +1471,26 @@
     </row>
     <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
-      <c r="K16" s="34" t="s">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+      <c r="K16" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="36"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="39"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
@@ -1554,12 +1555,12 @@
       <c r="D18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
       <c r="K18" s="22" t="s">
         <v>4</v>
       </c>
@@ -1654,16 +1655,16 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="41"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="36"/>
       <c r="K21" s="22" t="s">
         <v>4</v>
       </c>
@@ -1770,12 +1771,12 @@
       <c r="D24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="41"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="36"/>
       <c r="K24" s="22" t="s">
         <v>4</v>
       </c>
@@ -1870,16 +1871,16 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="41"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="36"/>
       <c r="K27" s="22" t="s">
         <v>4</v>
       </c>
@@ -1907,26 +1908,26 @@
     </row>
     <row r="29" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="39"/>
-      <c r="K30" s="37" t="s">
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="42"/>
+      <c r="K30" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="38"/>
-      <c r="P30" s="38"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="39"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="42"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
@@ -2230,21 +2231,21 @@
       <c r="E38" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="40" t="s">
+      <c r="F38" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="40"/>
-      <c r="H38" s="41"/>
-      <c r="K38" s="42" t="s">
+      <c r="G38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="K38" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="L38" s="40"/>
-      <c r="M38" s="40"/>
-      <c r="N38" s="40"/>
-      <c r="O38" s="40"/>
-      <c r="P38" s="40"/>
-      <c r="Q38" s="40"/>
-      <c r="R38" s="41"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="36"/>
     </row>
     <row r="39" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
@@ -2315,49 +2316,49 @@
       </c>
     </row>
     <row r="41" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="41"/>
-      <c r="K41" s="42" t="s">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36"/>
+      <c r="K41" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40"/>
-      <c r="N41" s="40"/>
-      <c r="O41" s="40"/>
-      <c r="P41" s="40"/>
-      <c r="Q41" s="40"/>
-      <c r="R41" s="41"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="36"/>
     </row>
     <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="44" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="36"/>
-      <c r="K44" s="37" t="s">
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="39"/>
+      <c r="K44" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="L44" s="38"/>
-      <c r="M44" s="38"/>
-      <c r="N44" s="38"/>
-      <c r="O44" s="38"/>
-      <c r="P44" s="38"/>
-      <c r="Q44" s="38"/>
-      <c r="R44" s="39"/>
+      <c r="L44" s="41"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="41"/>
+      <c r="P44" s="41"/>
+      <c r="Q44" s="41"/>
+      <c r="R44" s="42"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
@@ -2434,16 +2435,16 @@
       <c r="H46" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="K46" s="42" t="s">
+      <c r="K46" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="L46" s="40"/>
-      <c r="M46" s="40"/>
-      <c r="N46" s="40"/>
-      <c r="O46" s="40"/>
-      <c r="P46" s="40"/>
-      <c r="Q46" s="40"/>
-      <c r="R46" s="41"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="35"/>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="35"/>
+      <c r="R46" s="36"/>
     </row>
     <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="24"/>
@@ -2538,16 +2539,16 @@
       <c r="H49" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K49" s="42" t="s">
+      <c r="K49" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="L49" s="40"/>
-      <c r="M49" s="40"/>
-      <c r="N49" s="40"/>
-      <c r="O49" s="40"/>
-      <c r="P49" s="40"/>
-      <c r="Q49" s="40"/>
-      <c r="R49" s="41"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="35"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="35"/>
+      <c r="P49" s="35"/>
+      <c r="Q49" s="35"/>
+      <c r="R49" s="36"/>
     </row>
     <row r="50" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="24"/>
@@ -2642,16 +2643,16 @@
       <c r="H52" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="K52" s="42" t="s">
+      <c r="K52" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="L52" s="40"/>
-      <c r="M52" s="40"/>
-      <c r="N52" s="40"/>
-      <c r="O52" s="40"/>
-      <c r="P52" s="40"/>
-      <c r="Q52" s="40"/>
-      <c r="R52" s="41"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="35"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="35"/>
+      <c r="P52" s="35"/>
+      <c r="Q52" s="35"/>
+      <c r="R52" s="36"/>
     </row>
     <row r="53" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="24"/>
@@ -2746,29 +2747,29 @@
       <c r="H55" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K55" s="42" t="s">
+      <c r="K55" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="L55" s="40"/>
-      <c r="M55" s="40"/>
-      <c r="N55" s="40"/>
-      <c r="O55" s="40"/>
-      <c r="P55" s="40"/>
-      <c r="Q55" s="40"/>
-      <c r="R55" s="41"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="35"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="35"/>
+      <c r="P55" s="35"/>
+      <c r="Q55" s="35"/>
+      <c r="R55" s="36"/>
     </row>
     <row r="58" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="59" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="34" t="s">
+      <c r="A59" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="36"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="39"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
@@ -2946,15 +2947,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="K52:R52"/>
-    <mergeCell ref="K55:R55"/>
-    <mergeCell ref="K49:R49"/>
-    <mergeCell ref="K46:R46"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="K30:R30"/>
-    <mergeCell ref="K41:R41"/>
-    <mergeCell ref="K38:R38"/>
-    <mergeCell ref="K44:R44"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="K1:R1"/>
     <mergeCell ref="K16:R16"/>
@@ -2971,6 +2963,15 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A12:H12"/>
+    <mergeCell ref="K52:R52"/>
+    <mergeCell ref="K55:R55"/>
+    <mergeCell ref="K49:R49"/>
+    <mergeCell ref="K46:R46"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="K30:R30"/>
+    <mergeCell ref="K41:R41"/>
+    <mergeCell ref="K38:R38"/>
+    <mergeCell ref="K44:R44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2978,7 +2979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2988,16 +2989,16 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
@@ -3239,16 +3240,16 @@
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
@@ -3488,16 +3489,16 @@
     </row>
     <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
@@ -3586,16 +3587,16 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="36"/>
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
@@ -3694,29 +3695,29 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="41"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="36"/>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="36"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="39"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
@@ -3972,11 +3973,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H43" workbookViewId="0">
-      <selection activeCell="P69" sqref="P69"/>
+    <sheetView tabSelected="1" topLeftCell="H37" workbookViewId="0">
+      <selection activeCell="T57" sqref="T57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3990,36 +3991,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39"/>
-      <c r="K1" s="37" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
+      <c r="K1" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="39"/>
-      <c r="U1" s="37" t="s">
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="42"/>
+      <c r="U1" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="39"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="42"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
@@ -4553,26 +4554,26 @@
     </row>
     <row r="14" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39"/>
-      <c r="K15" s="37" t="s">
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="42"/>
+      <c r="K15" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="39"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="42"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
@@ -4960,26 +4961,26 @@
     </row>
     <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="39"/>
-      <c r="K29" s="37" t="s">
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="42"/>
+      <c r="K29" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
-      <c r="O29" s="38"/>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="38"/>
-      <c r="R29" s="39"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="42"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
@@ -5325,26 +5326,26 @@
     </row>
     <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="39"/>
-      <c r="K43" s="37" t="s">
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="42"/>
+      <c r="K43" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
-      <c r="O43" s="38"/>
-      <c r="P43" s="38"/>
-      <c r="Q43" s="38"/>
-      <c r="R43" s="39"/>
+      <c r="L43" s="41"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="41"/>
+      <c r="O43" s="41"/>
+      <c r="P43" s="41"/>
+      <c r="Q43" s="41"/>
+      <c r="R43" s="42"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
@@ -5709,31 +5710,11 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="U1:AB1"/>
-    <mergeCell ref="U3:AB3"/>
-    <mergeCell ref="U6:AB6"/>
-    <mergeCell ref="U9:AB9"/>
-    <mergeCell ref="U12:AB12"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="K9:R9"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="A43:H43"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A51:H51"/>
-    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="K48:R48"/>
+    <mergeCell ref="K43:R43"/>
+    <mergeCell ref="K45:R45"/>
+    <mergeCell ref="O54:R54"/>
+    <mergeCell ref="O51:R51"/>
     <mergeCell ref="K31:R31"/>
     <mergeCell ref="K34:R34"/>
     <mergeCell ref="K37:R37"/>
@@ -5744,13 +5725,47 @@
     <mergeCell ref="K23:R23"/>
     <mergeCell ref="K26:R26"/>
     <mergeCell ref="K29:R29"/>
-    <mergeCell ref="K48:R48"/>
-    <mergeCell ref="K43:R43"/>
-    <mergeCell ref="K45:R45"/>
-    <mergeCell ref="O54:R54"/>
-    <mergeCell ref="O51:R51"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A51:H51"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="K9:R9"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="U3:AB3"/>
+    <mergeCell ref="U6:AB6"/>
+    <mergeCell ref="U9:AB9"/>
+    <mergeCell ref="U12:AB12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B938E-6AB5-42FD-B378-F5907C784EC1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>